<commit_message>
Update model guide to include compensation calculations and 500 plus plan
</commit_message>
<xml_diff>
--- a/500PlusPlan/500PlusPlanCosts.xlsx
+++ b/500PlusPlan/500PlusPlanCosts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCoding2\500PlusPlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E8ED79-36FA-4F1D-B87A-5FA3C77FED29}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62C340C-E099-4B8B-B8BA-6A1AE20DF046}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11475" xr2:uid="{95F8874B-1661-4F8A-9599-69693F490963}"/>
   </bookViews>
@@ -96,15 +96,9 @@
     <t>Mid</t>
   </si>
   <si>
-    <t>Cost ($ Mill) to Purchase Target Water Volume (maf)</t>
-  </si>
-  <si>
     <t>Estimate the cost ($ million) by multiplying recent water prices ($/acre-foot) throughout the Colorado River basin (Table 1) by the target water volume (million acre-feet)(Table 2).</t>
   </si>
   <si>
-    <t>Table 2. Cost ($ million) to purchase different target water volumes (maf) at different prices ($/acre-foot)</t>
-  </si>
-  <si>
     <t>This workbook tries to estimate the cost to purchase water for the 500-Plus Plan (Allhands, 2021). In the 500-Plus Plan, the Lower Basin states increase their conservation efforts by 500,000 acre-feet per year over their current Drought Contingecy Plan schedule by voluntarily purchase water from Lower Basin users.</t>
   </si>
   <si>
@@ -112,6 +106,12 @@
   </si>
   <si>
     <t>Estimates consider uncertainties in the purchase price ($/acre-foot) and the target water volume (0.25, 0.5, and 1.0 maf per year).</t>
+  </si>
+  <si>
+    <t>Cost ($ Mill) to Purchase Target Water Volume (maf per year)</t>
+  </si>
+  <si>
+    <t>Table 2. Compensation ($ million) for different water prices ($/acre-foot) and different planned target water volumes (maf per year)</t>
   </si>
 </sst>
 </file>
@@ -124,7 +124,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,8 +160,15 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -186,6 +193,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -346,14 +365,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -366,19 +382,7 @@
     <xf numFmtId="6" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -400,32 +404,41 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="7"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -434,6 +447,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF0000FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -744,56 +762,56 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{552571F0-DC88-4C65-95FE-F2847390B80C}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="48.28515625" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>27</v>
+      <c r="A1" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="18"/>
-      <c r="B11" s="4" t="s">
+      <c r="A11" s="13"/>
+      <c r="B11" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -801,7 +819,7 @@
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -809,7 +827,7 @@
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -817,7 +835,7 @@
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -825,201 +843,201 @@
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="5">
         <v>2000</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
+      <c r="A18" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
     </row>
     <row r="19" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19" s="25"/>
-      <c r="F19" s="26"/>
+      <c r="D19" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="24"/>
+      <c r="F19" s="25"/>
     </row>
     <row r="20" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="9" t="s">
+      <c r="A20" s="18"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="F20" s="15" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="2">
+      <c r="A21" s="18"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="15">
         <v>0.25</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="17">
         <v>0.5</v>
       </c>
-      <c r="F21" s="11">
+      <c r="F21" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="13">
+      <c r="C22" s="8">
         <f>AVERAGE(100, 250)</f>
         <v>175</v>
       </c>
-      <c r="D22" s="14">
+      <c r="D22" s="9">
         <f t="shared" ref="D22:F27" si="0">$C22*D$21</f>
         <v>43.75</v>
       </c>
-      <c r="E22" s="15">
+      <c r="E22" s="10">
         <f t="shared" si="0"/>
         <v>87.5</v>
       </c>
-      <c r="F22" s="14">
+      <c r="F22" s="9">
         <f t="shared" si="0"/>
         <v>175</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="13">
+      <c r="C23" s="8">
         <v>300</v>
       </c>
-      <c r="D23" s="14">
+      <c r="D23" s="9">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-      <c r="E23" s="15">
+      <c r="E23" s="10">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
-      <c r="F23" s="14">
+      <c r="F23" s="9">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="12" t="str">
+      <c r="A24" s="7" t="str">
         <f>A23</f>
         <v>Upper Basin - Agriculture</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="13">
+      <c r="C24" s="8">
         <v>500</v>
       </c>
-      <c r="D24" s="14">
+      <c r="D24" s="9">
         <f t="shared" si="0"/>
         <v>125</v>
       </c>
-      <c r="E24" s="15">
+      <c r="E24" s="10">
         <f t="shared" si="0"/>
         <v>250</v>
       </c>
-      <c r="F24" s="14">
+      <c r="F24" s="9">
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="13">
+      <c r="C25" s="8">
         <v>700</v>
       </c>
-      <c r="D25" s="14">
+      <c r="D25" s="9">
         <f t="shared" si="0"/>
         <v>175</v>
       </c>
-      <c r="E25" s="15">
+      <c r="E25" s="10">
         <f t="shared" si="0"/>
         <v>350</v>
       </c>
-      <c r="F25" s="14">
+      <c r="F25" s="9">
         <f t="shared" si="0"/>
         <v>700</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="str">
+      <c r="A26" s="7" t="str">
         <f>A25</f>
         <v>Lower Basin - Agriculture</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="13">
+      <c r="C26" s="8">
         <v>1000</v>
       </c>
-      <c r="D26" s="14">
+      <c r="D26" s="9">
         <f t="shared" si="0"/>
         <v>250</v>
       </c>
-      <c r="E26" s="15">
+      <c r="E26" s="10">
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
-      <c r="F26" s="14">
+      <c r="F26" s="9">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="13">
+      <c r="C27" s="8">
         <v>2000</v>
       </c>
-      <c r="D27" s="14">
+      <c r="D27" s="9">
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
-      <c r="E27" s="15">
+      <c r="E27" s="10">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="F27" s="14">
+      <c r="F27" s="9">
         <f t="shared" si="0"/>
         <v>2000</v>
       </c>

</xml_diff>

<commit_message>
Update Model Guide with participants not parties. Other editing too.
</commit_message>
<xml_diff>
--- a/500PlusPlan/500PlusPlanCosts.xlsx
+++ b/500PlusPlan/500PlusPlanCosts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20379"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20385"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCoding2\500PlusPlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62C340C-E099-4B8B-B8BA-6A1AE20DF046}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D182DC83-87C2-44D5-A6B2-EC76BEAD63DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11475" xr2:uid="{95F8874B-1661-4F8A-9599-69693F490963}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11480" xr2:uid="{95F8874B-1661-4F8A-9599-69693F490963}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>Description</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>Table 2. Compensation ($ million) for different water prices ($/acre-foot) and different planned target water volumes (maf per year)</t>
+  </si>
+  <si>
+    <t>500 Plus Plan (Alhands, 2021)</t>
   </si>
 </sst>
 </file>
@@ -398,47 +401,47 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="7"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="7"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -760,62 +763,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{552571F0-DC88-4C65-95FE-F2847390B80C}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:A21"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="48.28515625" customWidth="1"/>
+    <col min="1" max="1" width="48.26953125" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" customWidth="1"/>
+    <col min="4" max="4" width="22.453125" customWidth="1"/>
+    <col min="5" max="5" width="19.54296875" customWidth="1"/>
+    <col min="6" max="6" width="23.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="A10" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="13"/>
+    <row r="11" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="16"/>
       <c r="B11" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
@@ -823,221 +826,229 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B14" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+    <row r="15" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B15" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+    <row r="16" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B16" s="5">
         <v>2000</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+    <row r="19" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-    </row>
-    <row r="19" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+    </row>
+    <row r="20" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B20" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C20" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="23" t="s">
+      <c r="D20" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="24"/>
-      <c r="F19" s="25"/>
-    </row>
-    <row r="20" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="15" t="s">
+      <c r="E20" s="23"/>
+      <c r="F20" s="24"/>
+    </row>
+    <row r="21" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="17"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="17" t="s">
+      <c r="E21" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F20" s="15" t="s">
+      <c r="F21" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="15">
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="17"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="12">
         <v>0.25</v>
       </c>
-      <c r="E21" s="17">
+      <c r="E22" s="14">
         <v>0.5</v>
       </c>
-      <c r="F21" s="16">
+      <c r="F22" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B23" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C23" s="8">
         <f>AVERAGE(100, 250)</f>
         <v>175</v>
       </c>
-      <c r="D22" s="9">
-        <f t="shared" ref="D22:F27" si="0">$C22*D$21</f>
+      <c r="D23" s="9">
+        <f t="shared" ref="D23:F28" si="0">$C23*D$22</f>
         <v>43.75</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E23" s="10">
         <f t="shared" si="0"/>
         <v>87.5</v>
       </c>
-      <c r="F22" s="9">
+      <c r="F23" s="9">
         <f t="shared" si="0"/>
         <v>175</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+    <row r="24" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B24" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C24" s="8">
         <v>300</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D24" s="9">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-      <c r="E23" s="10">
+      <c r="E24" s="10">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
-      <c r="F23" s="9">
+      <c r="F24" s="9">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="str">
-        <f>A23</f>
+    <row r="25" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="7" t="str">
+        <f>A24</f>
         <v>Upper Basin - Agriculture</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B25" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C25" s="8">
         <v>500</v>
       </c>
-      <c r="D24" s="9">
+      <c r="D25" s="9">
         <f t="shared" si="0"/>
         <v>125</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E25" s="10">
         <f t="shared" si="0"/>
         <v>250</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F25" s="9">
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+    <row r="26" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B26" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C26" s="8">
         <v>700</v>
       </c>
-      <c r="D25" s="9">
+      <c r="D26" s="9">
         <f t="shared" si="0"/>
         <v>175</v>
       </c>
-      <c r="E25" s="10">
+      <c r="E26" s="10">
         <f t="shared" si="0"/>
         <v>350</v>
       </c>
-      <c r="F25" s="9">
+      <c r="F26" s="9">
         <f t="shared" si="0"/>
         <v>700</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="str">
-        <f>A25</f>
+    <row r="27" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="7" t="str">
+        <f>A26</f>
         <v>Lower Basin - Agriculture</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B27" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C27" s="8">
         <v>1000</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D27" s="9">
         <f t="shared" si="0"/>
         <v>250</v>
       </c>
-      <c r="E26" s="10">
+      <c r="E27" s="10">
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
-      <c r="F26" s="9">
+      <c r="F27" s="9">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
+    <row r="28" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B28" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C28" s="8">
         <v>2000</v>
       </c>
-      <c r="D27" s="9">
+      <c r="D28" s="9">
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
-      <c r="E27" s="10">
+      <c r="E28" s="10">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="F27" s="9">
+      <c r="F28" s="9">
         <f t="shared" si="0"/>
         <v>2000</v>
       </c>
@@ -1045,11 +1056,11 @@
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="A18:F18"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="A19:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Tables 7 and 8 in Model Guide to list source for Upper and Lower Basin prices and include 2 and 4 maf goals
</commit_message>
<xml_diff>
--- a/500PlusPlan/500PlusPlanCosts.xlsx
+++ b/500PlusPlan/500PlusPlanCosts.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20385"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20387"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCoding2\500PlusPlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D182DC83-87C2-44D5-A6B2-EC76BEAD63DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA9A1CD-A2DF-425B-A271-C96BDF508760}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11480" xr2:uid="{95F8874B-1661-4F8A-9599-69693F490963}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="August 2022" sheetId="2" r:id="rId1"/>
+    <sheet name="500 Plus Plan" sheetId="1" r:id="rId2"/>
+    <sheet name="Combined" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="43">
   <si>
     <t>Description</t>
   </si>
@@ -115,19 +117,59 @@
   </si>
   <si>
     <t>500 Plus Plan (Alhands, 2021)</t>
+  </si>
+  <si>
+    <t>Price ($/acre-foot)</t>
+  </si>
+  <si>
+    <t>Upper Basin Agriculture</t>
+  </si>
+  <si>
+    <t>Lower Basin Agriculture</t>
+  </si>
+  <si>
+    <t>Cost to purchase 1, 2, and 4 million-acre-feet of conservation</t>
+  </si>
+  <si>
+    <t>Table 2. Compensation ($ billion) for different water prices and target water conservation volumes</t>
+  </si>
+  <si>
+    <t>Desalination in Sea of Cortez (James, 2021)</t>
+  </si>
+  <si>
+    <t>500 Plus Plan (Hager, 2021)</t>
+  </si>
+  <si>
+    <t>Upper Basin Agriculture*</t>
+  </si>
+  <si>
+    <t>Lower Basin Agriculture*</t>
+  </si>
+  <si>
+    <t>August 2022 goal</t>
+  </si>
+  <si>
+    <t>*Discussion with managers during basin account activity</t>
+  </si>
+  <si>
+    <t>Upper Basin agriculture*</t>
+  </si>
+  <si>
+    <t>Lower Basin agriculture*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,6 +212,19 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -209,7 +264,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -363,12 +418,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -410,6 +474,19 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="7"/>
     </xf>
@@ -442,6 +519,35 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="7"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -762,11 +868,237 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F273B223-3368-4D30-8DBD-76040D02CFA0}">
+  <dimension ref="A1:G26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="46.36328125" customWidth="1"/>
+    <col min="2" max="2" width="13.90625" customWidth="1"/>
+    <col min="3" max="3" width="39.36328125" customWidth="1"/>
+    <col min="4" max="4" width="5.81640625" customWidth="1"/>
+    <col min="5" max="5" width="6.453125" customWidth="1"/>
+    <col min="6" max="6" width="23.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="A10" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="21"/>
+      <c r="B11" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="5">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="34"/>
+    </row>
+    <row r="19" spans="1:7" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+    </row>
+    <row r="20" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="19" t="str">
+        <f t="shared" ref="D20:E20" si="0">TEXT(D26,"0")&amp;" maf"</f>
+        <v>2 maf</v>
+      </c>
+      <c r="E20" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>4 maf</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="8">
+        <f>$B$13</f>
+        <v>200</v>
+      </c>
+      <c r="C21" s="7" t="str">
+        <f>A12&amp;"; "&amp;A13</f>
+        <v>Pilot System Conservation Program (USBR, 2021e); 500 Plus Plan (Hager, 2021)</v>
+      </c>
+      <c r="D21" s="15">
+        <f t="shared" ref="D21:E24" si="1">$G21*D$26/1000</f>
+        <v>0.4</v>
+      </c>
+      <c r="E21" s="15">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="G21" s="8">
+        <f>$B$13</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B22" s="8">
+        <v>400</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="15">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="E22" s="15">
+        <f t="shared" si="1"/>
+        <v>1.6</v>
+      </c>
+      <c r="G22" s="8">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B23" s="8">
+        <f>AVERAGE(700,1000)</f>
+        <v>850</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="15">
+        <f t="shared" si="1"/>
+        <v>1.7</v>
+      </c>
+      <c r="E23" s="15">
+        <f t="shared" si="1"/>
+        <v>3.4</v>
+      </c>
+      <c r="G23" s="8">
+        <f>AVERAGE(700,1000)</f>
+        <v>850</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="8">
+        <v>2000</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="15">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E24" s="15">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="G24" s="8">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D26" s="17">
+        <v>2</v>
+      </c>
+      <c r="E26" s="17">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A17:B17"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{552571F0-DC88-4C65-95FE-F2847390B80C}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:B16"/>
+    <sheetView topLeftCell="A8" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -805,7 +1137,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="20" t="s">
         <v>0</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -813,7 +1145,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="16"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="3" t="s">
         <v>2</v>
       </c>
@@ -859,35 +1191,35 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
     </row>
     <row r="20" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="22" t="s">
+      <c r="D20" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="23"/>
-      <c r="F20" s="24"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="29"/>
     </row>
     <row r="21" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="17"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="20"/>
+      <c r="A21" s="22"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="25"/>
       <c r="D21" s="12" t="s">
         <v>13</v>
       </c>
@@ -899,9 +1231,9 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="17"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="21"/>
+      <c r="A22" s="22"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="26"/>
       <c r="D22" s="12">
         <v>0.25</v>
       </c>
@@ -1064,4 +1396,286 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3C41339-2860-47AA-AFF7-74689DA51AB1}">
+  <dimension ref="A1:H27"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="46.36328125" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" customWidth="1"/>
+    <col min="3" max="3" width="39.36328125" customWidth="1"/>
+    <col min="4" max="4" width="8.36328125" customWidth="1"/>
+    <col min="5" max="5" width="6.26953125" customWidth="1"/>
+    <col min="6" max="6" width="6.453125" customWidth="1"/>
+    <col min="7" max="7" width="4.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+      <c r="A10" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+      <c r="A11" s="37"/>
+      <c r="B11" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="A12" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="40" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="41">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="40" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="40" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="41">
+        <v>2000</v>
+      </c>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="34"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+    </row>
+    <row r="19" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+    </row>
+    <row r="20" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="33"/>
+      <c r="G20" s="18"/>
+    </row>
+    <row r="21" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="19" t="str">
+        <f>TEXT(D27,"0.0")&amp;" maf"</f>
+        <v>0.5 maf</v>
+      </c>
+      <c r="E21" s="19" t="str">
+        <f t="shared" ref="E21:F21" si="0">TEXT(E27,"0")&amp;" maf"</f>
+        <v>2 maf</v>
+      </c>
+      <c r="F21" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>4 maf</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="8">
+        <f>$B$13</f>
+        <v>200</v>
+      </c>
+      <c r="C22" s="7" t="str">
+        <f>A12&amp;"; "&amp;A13</f>
+        <v>Pilot System Conservation Program (USBR, 2021e); 500 Plus Plan (Hager, 2021)</v>
+      </c>
+      <c r="D22" s="15">
+        <f>$H22*D$27/1000</f>
+        <v>0.1</v>
+      </c>
+      <c r="E22" s="15">
+        <f>$H22*E$27/1000</f>
+        <v>0.4</v>
+      </c>
+      <c r="F22" s="15">
+        <f>$H22*F$27/1000</f>
+        <v>0.8</v>
+      </c>
+      <c r="H22" s="8">
+        <f>$B$13</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B23" s="8">
+        <v>400</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="15">
+        <f>$H23*D$27/1000</f>
+        <v>0.2</v>
+      </c>
+      <c r="E23" s="15">
+        <f>$H23*E$27/1000</f>
+        <v>0.8</v>
+      </c>
+      <c r="F23" s="15">
+        <f>$H23*F$27/1000</f>
+        <v>1.6</v>
+      </c>
+      <c r="H23" s="8">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B24" s="8">
+        <f>AVERAGE(700,1000)</f>
+        <v>850</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="15">
+        <f>$H24*D$27/1000</f>
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="E24" s="15">
+        <f>$H24*E$27/1000</f>
+        <v>1.7</v>
+      </c>
+      <c r="F24" s="15">
+        <f>$H24*F$27/1000</f>
+        <v>3.4</v>
+      </c>
+      <c r="H24" s="8">
+        <f>AVERAGE(700,1000)</f>
+        <v>850</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="8">
+        <v>2000</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="15">
+        <f>$H25*D$27/1000</f>
+        <v>1</v>
+      </c>
+      <c r="E25" s="15">
+        <f>$H25*E$27/1000</f>
+        <v>4</v>
+      </c>
+      <c r="F25" s="15">
+        <f>$H25*F$27/1000</f>
+        <v>8</v>
+      </c>
+      <c r="H25" s="8">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B26" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D27" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="E27" s="17">
+        <v>2</v>
+      </c>
+      <c r="F27" s="17">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="A17:B17"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Save tables as bitmap to show online
</commit_message>
<xml_diff>
--- a/500PlusPlan/500PlusPlanCosts.xlsx
+++ b/500PlusPlan/500PlusPlanCosts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCoding2\500PlusPlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA9A1CD-A2DF-425B-A271-C96BDF508760}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B23009-DD2F-4E35-B51E-9D10FD25C1C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11480" xr2:uid="{95F8874B-1661-4F8A-9599-69693F490963}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11480" activeTab="2" xr2:uid="{95F8874B-1661-4F8A-9599-69693F490963}"/>
   </bookViews>
   <sheets>
     <sheet name="August 2022" sheetId="2" r:id="rId1"/>
@@ -487,57 +487,12 @@
     <xf numFmtId="1" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="7"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="7"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="7"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -547,6 +502,51 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="6" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="7"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="7"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="7"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -869,20 +869,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F273B223-3368-4D30-8DBD-76040D02CFA0}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView topLeftCell="A18" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="46.36328125" customWidth="1"/>
     <col min="2" max="2" width="13.90625" customWidth="1"/>
-    <col min="3" max="3" width="39.36328125" customWidth="1"/>
-    <col min="4" max="4" width="5.81640625" customWidth="1"/>
+    <col min="3" max="3" width="13.08984375" customWidth="1"/>
+    <col min="4" max="4" width="39" customWidth="1"/>
     <col min="5" max="5" width="6.453125" customWidth="1"/>
-    <col min="6" max="6" width="23.26953125" customWidth="1"/>
+    <col min="6" max="6" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -911,7 +911,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="27" t="s">
         <v>0</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -919,7 +919,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="21"/>
+      <c r="A11" s="28"/>
       <c r="B11" s="3" t="s">
         <v>2</v>
       </c>
@@ -964,123 +964,123 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="34" t="s">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="34"/>
-    </row>
-    <row r="19" spans="1:7" ht="34" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="18" t="s">
+      <c r="B17" s="29"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C19" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="18"/>
       <c r="D19" s="18"/>
       <c r="E19" s="18"/>
       <c r="F19" s="18"/>
-    </row>
-    <row r="20" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="16" t="s">
+      <c r="G19" s="18"/>
+    </row>
+    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.35">
+      <c r="C20" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="D20" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="19" t="str">
-        <f t="shared" ref="D20:E20" si="0">TEXT(D26,"0")&amp;" maf"</f>
+      <c r="E20" s="19" t="str">
+        <f t="shared" ref="E20:F20" si="0">TEXT(E26,"0")&amp;" maf"</f>
         <v>2 maf</v>
       </c>
-      <c r="E20" s="19" t="str">
+      <c r="F20" s="19" t="str">
         <f t="shared" si="0"/>
         <v>4 maf</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="8">
+    <row r="21" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="C21" s="8">
         <f>$B$13</f>
         <v>200</v>
       </c>
-      <c r="C21" s="7" t="str">
+      <c r="D21" s="7" t="str">
         <f>A12&amp;"; "&amp;A13</f>
         <v>Pilot System Conservation Program (USBR, 2021e); 500 Plus Plan (Hager, 2021)</v>
       </c>
-      <c r="D21" s="15">
-        <f t="shared" ref="D21:E24" si="1">$G21*D$26/1000</f>
+      <c r="E21" s="15">
+        <f>$H21*E$26/1000</f>
         <v>0.4</v>
       </c>
-      <c r="E21" s="15">
-        <f t="shared" si="1"/>
+      <c r="F21" s="15">
+        <f>$H21*F$26/1000</f>
         <v>0.8</v>
       </c>
-      <c r="G21" s="8">
+      <c r="H21" s="8">
         <f>$B$13</f>
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B22" s="8">
+    <row r="22" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C22" s="8">
         <v>400</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="D22" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="15">
-        <f t="shared" si="1"/>
+      <c r="E22" s="15">
+        <f>$H22*E$26/1000</f>
         <v>0.8</v>
       </c>
-      <c r="E22" s="15">
-        <f t="shared" si="1"/>
+      <c r="F22" s="15">
+        <f>$H22*F$26/1000</f>
         <v>1.6</v>
       </c>
-      <c r="G22" s="8">
+      <c r="H22" s="8">
         <v>400</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B23" s="8">
+    <row r="23" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C23" s="8">
         <f>AVERAGE(700,1000)</f>
         <v>850</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="D23" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="15">
-        <f t="shared" si="1"/>
+      <c r="E23" s="15">
+        <f>$H23*E$26/1000</f>
         <v>1.7</v>
       </c>
-      <c r="E23" s="15">
-        <f t="shared" si="1"/>
+      <c r="F23" s="15">
+        <f>$H23*F$26/1000</f>
         <v>3.4</v>
       </c>
-      <c r="G23" s="8">
+      <c r="H23" s="8">
         <f>AVERAGE(700,1000)</f>
         <v>850</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="8">
+    <row r="24" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+      <c r="C24" s="8">
         <v>2000</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="D24" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D24" s="15">
-        <f t="shared" si="1"/>
+      <c r="E24" s="15">
+        <f>$H24*E$26/1000</f>
         <v>4</v>
       </c>
-      <c r="E24" s="15">
-        <f t="shared" si="1"/>
+      <c r="F24" s="15">
+        <f>$H24*F$26/1000</f>
         <v>8</v>
       </c>
-      <c r="G24" s="8">
+      <c r="H24" s="8">
         <v>2000</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D26" s="17">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E26" s="17">
         <v>2</v>
       </c>
-      <c r="E26" s="17">
+      <c r="F26" s="17">
         <v>4</v>
       </c>
     </row>
@@ -1137,7 +1137,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="27" t="s">
         <v>0</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1145,7 +1145,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="21"/>
+      <c r="A11" s="28"/>
       <c r="B11" s="3" t="s">
         <v>2</v>
       </c>
@@ -1191,35 +1191,35 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="30" t="s">
+      <c r="A19" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
     </row>
     <row r="20" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="C20" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="27" t="s">
+      <c r="D20" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="28"/>
-      <c r="F20" s="29"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="37"/>
     </row>
     <row r="21" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="22"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="25"/>
+      <c r="A21" s="30"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="33"/>
       <c r="D21" s="12" t="s">
         <v>13</v>
       </c>
@@ -1231,9 +1231,9 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="22"/>
-      <c r="B22" s="23"/>
-      <c r="C22" s="26"/>
+      <c r="A22" s="30"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="34"/>
       <c r="D22" s="12">
         <v>0.25</v>
       </c>
@@ -1402,14 +1402,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3C41339-2860-47AA-AFF7-74689DA51AB1}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:B17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="46.36328125" customWidth="1"/>
-    <col min="2" max="2" width="12.81640625" customWidth="1"/>
+    <col min="2" max="2" width="10.08984375" customWidth="1"/>
     <col min="3" max="3" width="39.36328125" customWidth="1"/>
     <col min="4" max="4" width="8.36328125" customWidth="1"/>
     <col min="5" max="5" width="6.26953125" customWidth="1"/>
@@ -1443,70 +1443,70 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.35">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="23" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.35">
-      <c r="A11" s="37"/>
-      <c r="B11" s="38" t="s">
+      <c r="A11" s="39"/>
+      <c r="B11" s="23" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="31" x14ac:dyDescent="0.35">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="25" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="41">
+      <c r="B13" s="26">
         <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="25" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="25" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="41">
+      <c r="B16" s="26">
         <v>2000</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="34"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
     </row>
     <row r="19" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="18" t="s">
@@ -1519,24 +1519,24 @@
       <c r="G19" s="18"/>
     </row>
     <row r="20" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="31" t="s">
+      <c r="C20" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="32" t="s">
+      <c r="D20" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="33" t="s">
+      <c r="E20" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="33"/>
+      <c r="F20" s="40"/>
       <c r="G20" s="18"/>
     </row>
     <row r="21" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="31"/>
-      <c r="C21" s="31"/>
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
       <c r="D21" s="19" t="str">
         <f>TEXT(D27,"0.0")&amp;" maf"</f>
         <v>0.5 maf</v>
@@ -1560,15 +1560,15 @@
         <v>Pilot System Conservation Program (USBR, 2021e); 500 Plus Plan (Hager, 2021)</v>
       </c>
       <c r="D22" s="15">
-        <f>$H22*D$27/1000</f>
+        <f t="shared" ref="D22:F25" si="1">$H22*D$27/1000</f>
         <v>0.1</v>
       </c>
       <c r="E22" s="15">
-        <f>$H22*E$27/1000</f>
+        <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
       <c r="F22" s="15">
-        <f>$H22*F$27/1000</f>
+        <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
       <c r="H22" s="8">
@@ -1584,15 +1584,15 @@
         <v>37</v>
       </c>
       <c r="D23" s="15">
-        <f>$H23*D$27/1000</f>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="E23" s="15">
-        <f>$H23*E$27/1000</f>
+        <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
       <c r="F23" s="15">
-        <f>$H23*F$27/1000</f>
+        <f t="shared" si="1"/>
         <v>1.6</v>
       </c>
       <c r="H23" s="8">
@@ -1608,15 +1608,15 @@
         <v>38</v>
       </c>
       <c r="D24" s="15">
-        <f>$H24*D$27/1000</f>
+        <f t="shared" si="1"/>
         <v>0.42499999999999999</v>
       </c>
       <c r="E24" s="15">
-        <f>$H24*E$27/1000</f>
+        <f t="shared" si="1"/>
         <v>1.7</v>
       </c>
       <c r="F24" s="15">
-        <f>$H24*F$27/1000</f>
+        <f t="shared" si="1"/>
         <v>3.4</v>
       </c>
       <c r="H24" s="8">
@@ -1632,15 +1632,15 @@
         <v>35</v>
       </c>
       <c r="D25" s="15">
-        <f>$H25*D$27/1000</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E25" s="15">
-        <f>$H25*E$27/1000</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="F25" s="15">
-        <f>$H25*F$27/1000</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="H25" s="8">
@@ -1648,13 +1648,13 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B26" s="34" t="s">
+      <c r="B26" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D27" s="17">

</xml_diff>